<commit_message>
changed LWX to be TB based instead of B based. also changed formatting for easier consumption
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Python Scripts\OIT Billing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aordal\oit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3323B41-08F7-4C71-A1F8-0C3B6A155DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA04C1E-FDBC-42C0-B055-6AE7A942B08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chargeback By Department" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Total Files</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>Total Capacity (TB)</t>
-  </si>
-  <si>
-    <t>Total Capacity (GiB)</t>
   </si>
   <si>
     <t xml:space="preserve">% Utilized </t>
@@ -278,20 +275,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -307,9 +298,19 @@
     <xf numFmtId="44" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -591,504 +592,425 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE3D3B3-9DB9-4A69-95AF-D4E7EB8BC937}">
-  <dimension ref="B2:J31"/>
+  <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="44" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E2" s="12" t="s">
+    <row r="2" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="E2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="13">
+      <c r="F5" s="11">
         <f>SUM(F3:F4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="16"/>
-    </row>
-    <row r="7" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
+    <row r="6" spans="2:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="B6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>33</v>
-      </c>
+      <c r="G7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3">
-        <f>E8*1000*(1/1.024^3)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="3" t="e">
-        <f>F8/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="5" t="e">
-        <f>F3*G8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="16"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19" t="e">
+        <f>E8/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="20" t="e">
+        <f>F3*F8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="3">
-        <f t="shared" ref="F9:F26" si="0">E9*1000*(1/1.024^3)</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="3" t="e">
-        <f>F9/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" s="5" t="e">
-        <f>F3*G9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="19" t="e">
+        <f>E9/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" s="20" t="e">
+        <f>F3*F9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="3" t="e">
-        <f>F10/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H10" s="5" t="e">
-        <f>G10*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="19" t="e">
+        <f>E10/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10" s="20" t="e">
+        <f>F3*F10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="3" t="e">
-        <f>F11/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H11" s="5" t="e">
-        <f>G11*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="19" t="e">
+        <f>E11/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="20" t="e">
+        <f>F3*F11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="3" t="e">
-        <f>F12/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H12" s="5" t="e">
-        <f>G12*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="19" t="e">
+        <f>E12/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" s="20" t="e">
+        <f>F3*F12</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="3" t="e">
-        <f>F13/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" s="5" t="e">
-        <f>G13*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="19" t="e">
+        <f>E13/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="20" t="e">
+        <f>F3*F13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="3" t="e">
-        <f>F14/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" s="5" t="e">
-        <f>G14*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="19" t="e">
+        <f>E14/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" s="20" t="e">
+        <f>F3*F14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="3" t="e">
-        <f>F15/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="5" t="e">
-        <f>G15*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="19" t="e">
+        <f>E15/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="20" t="e">
+        <f>F3*F15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="3" t="e">
-        <f>F16/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="5" t="e">
-        <f>G16*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="19" t="e">
+        <f>E16/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="20" t="e">
+        <f>F3*F16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="3" t="e">
-        <f>F17/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="5" t="e">
-        <f>G17*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="19" t="e">
+        <f>E17/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="20" t="e">
+        <f>F3*F17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="3" t="e">
-        <f>F18/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="5" t="e">
-        <f>G18*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="19" t="e">
+        <f>E18/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="20" t="e">
+        <f>F3*F18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="3" t="e">
-        <f>F19/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H19" s="5" t="e">
-        <f>G19*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="19" t="e">
+        <f>E19/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" s="20" t="e">
+        <f>F3*F19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="3" t="e">
-        <f>F20/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H20" s="5" t="e">
-        <f>G20*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="D20" s="16"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="19" t="e">
+        <f>E20/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" s="20" t="e">
+        <f>F3*F20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="3" t="e">
-        <f>F21/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H21" s="5" t="e">
-        <f>G21*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19" t="e">
+        <f>E21/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" s="20" t="e">
+        <f>F3*F21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="3" t="e">
-        <f>F22/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H22" s="5" t="e">
-        <f>G22*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19" t="e">
+        <f>E22/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" s="20" t="e">
+        <f>F3*F22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="3" t="e">
-        <f>F23/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H23" s="5" t="e">
-        <f>G23*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="19" t="e">
+        <f>E23/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" s="20" t="e">
+        <f>F3*F23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="3" t="e">
-        <f>F24/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H24" s="5" t="e">
-        <f>G24*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="19" t="e">
+        <f>E24/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G24" s="20" t="e">
+        <f>F3*F24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="3" t="e">
-        <f>F25/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H25" s="5" t="e">
-        <f>G25*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="19" t="e">
+        <f>E25/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G25" s="20" t="e">
+        <f>F3*F25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="3" t="e">
-        <f>F26/F27</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H26" s="5" t="e">
-        <f>G26*F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="19" t="e">
+        <f>E26/E27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G26" s="20" t="e">
+        <f>F3*F26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="7"/>
       <c r="C27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="10">
+        <v>33</v>
+      </c>
+      <c r="D27" s="8">
         <f>SUM(D8:D26)</f>
         <v>0</v>
       </c>
@@ -1096,43 +1018,39 @@
         <f>SUM(E8:E26)</f>
         <v>0</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="14" t="e">
         <f>SUM(F8:F26)</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="3" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G27" s="4" t="e">
         <f>SUM(G8:G26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H27" s="5" t="e">
-        <f>SUM(H8:H26)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B30" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="14"/>
-    </row>
-    <row r="31" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B31" s="11" t="s">
+    </row>
+    <row r="30" spans="2:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="B30" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="12"/>
+    </row>
+    <row r="31" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B31" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="E31" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>33</v>
+      <c r="F31" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>